<commit_message>
Changed names in Critical_appraisal_sheet.xlsx and removed redundant information in Critical_appraisal_EWAS_list.xlsx
</commit_message>
<xml_diff>
--- a/Data/Critical_appraisal_sheet.xlsx
+++ b/Data/Critical_appraisal_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc14dadc081973b4/Documenten/Documenten-UU/Master/MCLS/2022-2023/Writing_assignment/Data_visualization/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3396" documentId="8_{E2C065E7-D457-4A24-A390-EB089759AAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D63058F2-BEC6-46E7-9EF4-30C49AD1FA87}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB8C176B-DB0F-4D84-8376-CACF3FD9A6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{72E9CED1-2BD4-42A1-8B64-B8976DC4E720}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{72E9CED1-2BD4-42A1-8B64-B8976DC4E720}"/>
   </bookViews>
   <sheets>
     <sheet name="articles" sheetId="5" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3166" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3167" uniqueCount="550">
   <si>
     <t>key</t>
   </si>
@@ -1713,6 +1713,9 @@
   </si>
   <si>
     <t>Prediction_list</t>
+  </si>
+  <si>
+    <t>prediction</t>
   </si>
 </sst>
 </file>
@@ -3109,10 +3112,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="4" xr16:uid="{15CC8DA3-5F64-4EA0-8089-A8988075BC9C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="37" unboundColumnsRight="13">
@@ -3617,7 +3616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F4E436-D5D6-4EB4-91FE-E13DF1EFAE15}">
   <dimension ref="A1:P70"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
@@ -7151,10 +7150,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2002D060-E539-4BDD-A38E-FE6E68D8D0B5}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7327,11 +7326,6 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>517</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7345,7 +7339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A0C8B5B-3316-4394-8E67-1E87460A8AD1}">
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView topLeftCell="D43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="L71" sqref="L71"/>
     </sheetView>
   </sheetViews>
@@ -10975,8 +10969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44775334-D4BD-4DE5-A870-2F3B6E10CAEF}">
   <dimension ref="A1:H150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D126" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G150"/>
+    <sheetView topLeftCell="D126" workbookViewId="0">
+      <selection activeCell="E146" sqref="E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15010,10 +15004,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21031C4C-278D-4368-941C-9030DE7C41E7}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15028,6 +15022,14 @@
       </c>
       <c r="B1" t="s">
         <v>432</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="B2" t="s">
+        <v>517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>